<commit_message>
including lidar and lidar support
</commit_message>
<xml_diff>
--- a/RUR3/BOM.xlsx
+++ b/RUR3/BOM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{8422152E-367F-0841-815D-EFD5B23D9010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{84080BC2-D426-4C31-B171-26D0E98B07E5}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{8422152E-367F-0841-815D-EFD5B23D9010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{FB39DFFA-1180-4EBF-BA2F-4C351ADC184B}"/>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="3195" windowWidth="22125" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>link2-datablade</t>
+  </si>
+  <si>
+    <t>profile 20 x 40</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
   <dimension ref="B4:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,26 +1441,40 @@
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
       <c r="D29" s="1">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>116.84</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>233.68</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>116.84</v>
       </c>
       <c r="H29" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I29" s="1" t="b">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="4"/>
+        <v>233.68</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
@@ -1528,7 +1545,7 @@
     <row r="34" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J34" s="1">
         <f>SUM(J5:J33)</f>
-        <v>5511.2870000000003</v>
+        <v>5744.9670000000006</v>
       </c>
     </row>
   </sheetData>
@@ -1548,8 +1565,9 @@
     <hyperlink ref="M27" r:id="rId13" xr:uid="{6BE1BF31-761B-4AF0-8951-5C72AFC462C0}"/>
     <hyperlink ref="M28" r:id="rId14" xr:uid="{449A4F0B-A6C0-4F59-B961-12E43F889C46}"/>
     <hyperlink ref="N27" r:id="rId15" xr:uid="{DAE6C813-FF8A-4F50-9436-01028640B331}"/>
+    <hyperlink ref="M29" r:id="rId16" xr:uid="{3CD5B08E-EDDD-4295-8AE4-53158DDAAEB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>